<commit_message>
fix: upload data pekerja
</commit_message>
<xml_diff>
--- a/src/assets/template/Employee.xlsx
+++ b/src/assets/template/Employee.xlsx
@@ -22,7 +22,7 @@
     <t>NIP</t>
   </si>
   <si>
-    <t>PSADESC</t>
+    <t>UNITKERJA</t>
   </si>
   <si>
     <t>LEVELJABATAN</t>
@@ -60,13 +60,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,13 +76,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -102,98 +95,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,6 +154,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -215,31 +185,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,187 +253,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,8 +465,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -481,8 +504,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,6 +521,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,190 +559,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -719,73 +712,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Kepala 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Koma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Koma" xfId="3" builtinId="3"/>
-    <cellStyle name="Mata Uang [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="20% - Aksen4" xfId="5" builtinId="42"/>
-    <cellStyle name="Mata Uang" xfId="6" builtinId="4"/>
-    <cellStyle name="Sel Ditautkan" xfId="7" builtinId="24"/>
-    <cellStyle name="Persen" xfId="8" builtinId="5"/>
-    <cellStyle name="Kepala 4" xfId="9" builtinId="19"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="20% - Aksen6" xfId="11" builtinId="50"/>
-    <cellStyle name="Total" xfId="12" builtinId="25"/>
-    <cellStyle name="Hyperlink yang Diikuti" xfId="13" builtinId="9"/>
-    <cellStyle name="20% - Aksen2" xfId="14" builtinId="34"/>
-    <cellStyle name="Catatan" xfId="15" builtinId="10"/>
-    <cellStyle name="Teks Peringatan" xfId="16" builtinId="11"/>
-    <cellStyle name="Kepala 2" xfId="17" builtinId="17"/>
-    <cellStyle name="Judul" xfId="18" builtinId="15"/>
-    <cellStyle name="Aksen3" xfId="19" builtinId="37"/>
-    <cellStyle name="Teks CExplanatory" xfId="20" builtinId="53"/>
-    <cellStyle name="Kepala 1" xfId="21" builtinId="16"/>
-    <cellStyle name="60% - Aksen2" xfId="22" builtinId="36"/>
-    <cellStyle name="input" xfId="23" builtinId="20"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
     <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="Perhitungan" xfId="25" builtinId="22"/>
-    <cellStyle name="Cek Sel" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - Aksen5" xfId="27" builtinId="46"/>
-    <cellStyle name="Baik" xfId="28" builtinId="26"/>
-    <cellStyle name="Buruk" xfId="29" builtinId="27"/>
-    <cellStyle name="Netral" xfId="30" builtinId="28"/>
-    <cellStyle name="Aksen1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Aksen1" xfId="32" builtinId="30"/>
-    <cellStyle name="40% - Aksen1" xfId="33" builtinId="31"/>
-    <cellStyle name="60% - Aksen1" xfId="34" builtinId="32"/>
-    <cellStyle name="Aksen2" xfId="35" builtinId="33"/>
-    <cellStyle name="40% - Aksen2" xfId="36" builtinId="35"/>
-    <cellStyle name="20% - Aksen3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Aksen3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Aksen3" xfId="39" builtinId="40"/>
-    <cellStyle name="Aksen4" xfId="40" builtinId="41"/>
-    <cellStyle name="40% - Aksen4" xfId="41" builtinId="43"/>
-    <cellStyle name="60% - Aksen4" xfId="42" builtinId="44"/>
-    <cellStyle name="Aksen5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Aksen5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Aksen5" xfId="45" builtinId="48"/>
-    <cellStyle name="Aksen6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Aksen6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Aksen6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1057,7 +1050,7 @@
   <dimension ref="A1:AA131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>